<commit_message>
Initial USB Keyboard Example
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\EE345L Class\EE445LTeachingMaterials\0000_Spring2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\ece-445l-final-project-ad_jm_mj_ew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A28EEF-BE93-4159-9EEE-C41A6AAED890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E357A8DA-18B4-48D9-86EB-6B6E9BE622D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="1110" windowWidth="28740" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$5:$J$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$5:$J$150</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="523">
   <si>
     <t>Quantity</t>
   </si>
@@ -1671,6 +1671,42 @@
   </si>
   <si>
     <t>https://www.allelectronics.com/item/shs-40/1-x-40-header-0.1-spacing/1.html</t>
+  </si>
+  <si>
+    <t>Gateron</t>
+  </si>
+  <si>
+    <t>KS-9</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>65x RGB MX Type Key Switch</t>
+  </si>
+  <si>
+    <t>Custom 3D printed shell</t>
+  </si>
+  <si>
+    <t>TIW</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>BGM220PC22HNA Bluetooth Module</t>
+  </si>
+  <si>
+    <t>Silicon Labs</t>
+  </si>
+  <si>
+    <t>634-BGM220PC22HNA2R</t>
+  </si>
+  <si>
+    <t>BGM220PC22HNA2R</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -2249,28 +2285,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S148"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:S151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J161" sqref="J161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="11.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="3" customWidth="1"/>
+    <col min="2" max="3" width="11.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="18" style="3" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="23" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2288,7 +2326,7 @@
       </c>
       <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>471</v>
       </c>
@@ -2304,7 +2342,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -2316,7 +2354,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>232</v>
       </c>
@@ -2326,8 +2364,15 @@
       <c r="E4" s="11" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="J4" s="2">
+        <f>SUM(J5:J200)</f>
+        <v>80.83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2365,7 +2410,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -2398,7 +2443,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -2428,7 +2473,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -2462,7 +2507,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -2495,7 +2540,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -2531,7 +2576,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>0</v>
       </c>
@@ -2564,7 +2609,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>0</v>
       </c>
@@ -2594,7 +2639,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>0</v>
       </c>
@@ -2630,7 +2675,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>0</v>
       </c>
@@ -2660,7 +2705,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>0</v>
       </c>
@@ -2690,7 +2735,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>0</v>
       </c>
@@ -2714,7 +2759,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>0</v>
       </c>
@@ -2744,7 +2789,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>0</v>
       </c>
@@ -2774,7 +2819,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>0</v>
       </c>
@@ -2798,7 +2843,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>0</v>
       </c>
@@ -2822,7 +2867,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>0</v>
       </c>
@@ -2846,7 +2891,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>0</v>
       </c>
@@ -2870,7 +2915,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>0</v>
       </c>
@@ -2894,7 +2939,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>0</v>
       </c>
@@ -2918,7 +2963,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>0</v>
       </c>
@@ -2942,7 +2987,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>0</v>
       </c>
@@ -2981,7 +3026,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>0</v>
       </c>
@@ -3017,7 +3062,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>0</v>
       </c>
@@ -3047,7 +3092,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>0</v>
       </c>
@@ -3077,7 +3122,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>0</v>
       </c>
@@ -3107,7 +3152,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>0</v>
       </c>
@@ -3137,7 +3182,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>0</v>
       </c>
@@ -3167,7 +3212,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>0</v>
       </c>
@@ -3200,7 +3245,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>0</v>
       </c>
@@ -3233,28 +3278,34 @@
         <v>509</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>505</v>
+        <v>175</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>17</v>
+        <v>313</v>
       </c>
       <c r="I35" s="2">
-        <v>0.27</v>
+        <v>0.05</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>A35*I35</f>
+        <v>3.25</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>198</v>
@@ -3266,7 +3317,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>0</v>
       </c>
@@ -3292,7 +3343,7 @@
         <v>0.11</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="0"/>
+        <f>A36*I36</f>
         <v>0</v>
       </c>
       <c r="K36" s="1" t="s">
@@ -3302,7 +3353,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>0</v>
       </c>
@@ -3328,7 +3379,7 @@
         <v>0.23</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="0"/>
+        <f>A37*I37</f>
         <v>0</v>
       </c>
       <c r="K37" s="1" t="s">
@@ -3338,7 +3389,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>0</v>
       </c>
@@ -3364,7 +3415,7 @@
         <v>0.23</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" ref="J38:J73" si="1">A38*I38</f>
+        <f>A38*I38</f>
         <v>0</v>
       </c>
       <c r="K38" s="1" t="s">
@@ -3374,7 +3425,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>0</v>
       </c>
@@ -3400,7 +3451,7 @@
         <v>0.23</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="1"/>
+        <f>A39*I39</f>
         <v>0</v>
       </c>
       <c r="K39" s="1" t="s">
@@ -3410,7 +3461,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>0</v>
       </c>
@@ -3436,7 +3487,7 @@
         <v>0.23</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" si="1"/>
+        <f>A40*I40</f>
         <v>0</v>
       </c>
       <c r="K40" s="1" t="s">
@@ -3446,7 +3497,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>0</v>
       </c>
@@ -3482,7 +3533,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>0</v>
       </c>
@@ -3518,7 +3569,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>0</v>
       </c>
@@ -3544,7 +3595,7 @@
         <v>0.23</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="1"/>
+        <f>A43*I43</f>
         <v>0</v>
       </c>
       <c r="K43" s="1" t="s">
@@ -3554,7 +3605,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>0</v>
       </c>
@@ -3587,7 +3638,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>0</v>
       </c>
@@ -3613,7 +3664,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" si="1"/>
+        <f>A45*I45</f>
         <v>0</v>
       </c>
       <c r="K45" s="1" t="s">
@@ -3626,7 +3677,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>0</v>
       </c>
@@ -3652,7 +3703,7 @@
         <v>2.46</v>
       </c>
       <c r="J46" s="2">
-        <f t="shared" ref="J46:J52" si="2">A46*I46</f>
+        <f>A46*I46</f>
         <v>0</v>
       </c>
       <c r="K46" s="1" t="s">
@@ -3662,34 +3713,34 @@
         <v>239</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>454</v>
+        <v>47</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>451</v>
+        <v>55</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>453</v>
+        <v>31</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>267</v>
+        <v>11</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="I47" s="2">
-        <v>0.47</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J47" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>A47*I47</f>
+        <v>0.86999999999999988</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>455</v>
@@ -3698,7 +3749,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>0</v>
       </c>
@@ -3724,7 +3775,7 @@
         <v>0.65</v>
       </c>
       <c r="J48" s="2">
-        <f t="shared" si="2"/>
+        <f>A48*I48</f>
         <v>0</v>
       </c>
       <c r="K48" s="1" t="s">
@@ -3734,7 +3785,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>0</v>
       </c>
@@ -3760,7 +3811,7 @@
         <v>0.26</v>
       </c>
       <c r="J49" s="2">
-        <f t="shared" si="2"/>
+        <f>A49*I49</f>
         <v>0</v>
       </c>
       <c r="K49" s="1" t="s">
@@ -3770,7 +3821,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>0</v>
       </c>
@@ -3796,7 +3847,7 @@
         <v>0.27</v>
       </c>
       <c r="J50" s="2">
-        <f t="shared" si="2"/>
+        <f>A50*I50</f>
         <v>0</v>
       </c>
       <c r="K50" s="1" t="s">
@@ -3806,22 +3857,28 @@
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>367</v>
+        <v>505</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="I51" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.27</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>A51*I51</f>
+        <v>0.27</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>258</v>
@@ -3830,7 +3887,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>0</v>
       </c>
@@ -3856,7 +3913,7 @@
         <v>2.7</v>
       </c>
       <c r="J52" s="2">
-        <f t="shared" si="2"/>
+        <f>A52*I52</f>
         <v>0</v>
       </c>
       <c r="K52" s="1" t="s">
@@ -3866,34 +3923,34 @@
         <v>239</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>188</v>
+        <v>26</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>344</v>
+        <v>454</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>189</v>
+        <v>451</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>347</v>
+        <v>453</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>267</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>346</v>
+        <v>452</v>
       </c>
       <c r="I53" s="2">
-        <v>11.55</v>
+        <v>0.47</v>
       </c>
       <c r="J53" s="2">
         <f>A53*I53</f>
-        <v>0</v>
+        <v>0.47</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>345</v>
@@ -3902,7 +3959,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>0</v>
       </c>
@@ -3941,34 +3998,22 @@
         <v>465</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>313</v>
+        <v>26</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>367</v>
       </c>
       <c r="I55" s="2">
-        <v>0.05</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J55" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>A55*I55</f>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>173</v>
@@ -3977,7 +4022,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>0</v>
       </c>
@@ -4013,7 +4058,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>0</v>
       </c>
@@ -4049,7 +4094,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>0</v>
       </c>
@@ -4075,7 +4120,7 @@
         <v>0.19</v>
       </c>
       <c r="J58" s="2">
-        <f t="shared" si="1"/>
+        <f>A58*I58</f>
         <v>0</v>
       </c>
       <c r="K58" s="1" t="s">
@@ -4085,7 +4130,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>0</v>
       </c>
@@ -4111,7 +4156,7 @@
         <v>12.15</v>
       </c>
       <c r="J59" s="2">
-        <f t="shared" si="1"/>
+        <f>A59*I59</f>
         <v>0</v>
       </c>
       <c r="K59" s="1" t="s">
@@ -4121,7 +4166,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>0</v>
       </c>
@@ -4157,7 +4202,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>0</v>
       </c>
@@ -4183,7 +4228,7 @@
         <v>14.18</v>
       </c>
       <c r="J61" s="2">
-        <f t="shared" si="1"/>
+        <f>A61*I61</f>
         <v>0</v>
       </c>
       <c r="K61" s="3" t="s">
@@ -4193,7 +4238,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>0</v>
       </c>
@@ -4219,7 +4264,7 @@
         <v>9.09</v>
       </c>
       <c r="J62" s="2">
-        <f t="shared" si="1"/>
+        <f>A62*I62</f>
         <v>0</v>
       </c>
       <c r="K62" s="1" t="s">
@@ -4229,7 +4274,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>0</v>
       </c>
@@ -4249,7 +4294,7 @@
         <v>492</v>
       </c>
       <c r="J63" s="2">
-        <f t="shared" si="1"/>
+        <f>A63*I63</f>
         <v>0</v>
       </c>
       <c r="K63" s="3" t="s">
@@ -4262,7 +4307,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>0</v>
       </c>
@@ -4288,7 +4333,7 @@
         <v>3.06</v>
       </c>
       <c r="J64" s="2">
-        <f t="shared" si="1"/>
+        <f>A64*I64</f>
         <v>0</v>
       </c>
       <c r="K64" s="1" t="s">
@@ -4301,7 +4346,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>0</v>
       </c>
@@ -4340,7 +4385,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>0</v>
       </c>
@@ -4379,7 +4424,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>0</v>
       </c>
@@ -4405,7 +4450,7 @@
         <v>1.21</v>
       </c>
       <c r="J67" s="2">
-        <f t="shared" si="1"/>
+        <f>A67*I67</f>
         <v>0</v>
       </c>
       <c r="K67" s="1" t="s">
@@ -4418,7 +4463,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>0</v>
       </c>
@@ -4444,7 +4489,7 @@
         <v>3.5</v>
       </c>
       <c r="J68" s="2">
-        <f t="shared" si="1"/>
+        <f>A68*I68</f>
         <v>0</v>
       </c>
       <c r="K68" s="1" t="s">
@@ -4457,7 +4502,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>0</v>
       </c>
@@ -4477,7 +4522,7 @@
         <v>0.4</v>
       </c>
       <c r="J69" s="2">
-        <f t="shared" si="1"/>
+        <f>A69*I69</f>
         <v>0</v>
       </c>
       <c r="L69" s="1" t="s">
@@ -4487,7 +4532,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>0</v>
       </c>
@@ -4517,7 +4562,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>0</v>
       </c>
@@ -4550,7 +4595,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>0</v>
       </c>
@@ -4576,7 +4621,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="J72" s="2">
-        <f t="shared" si="1"/>
+        <f>A72*I72</f>
         <v>0</v>
       </c>
       <c r="K72" s="1" t="s">
@@ -4589,7 +4634,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>0</v>
       </c>
@@ -4609,7 +4654,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J73" s="2">
-        <f t="shared" si="1"/>
+        <f>A73*I73</f>
         <v>0</v>
       </c>
       <c r="K73" s="1" t="s">
@@ -4622,7 +4667,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>0</v>
       </c>
@@ -4642,7 +4687,7 @@
         <v>0.09</v>
       </c>
       <c r="J74" s="2">
-        <f t="shared" ref="J74:J116" si="3">A74*I74</f>
+        <f>A74*I74</f>
         <v>0</v>
       </c>
       <c r="K74" s="1" t="s">
@@ -4655,7 +4700,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>0</v>
       </c>
@@ -4675,7 +4720,7 @@
         <v>2.99</v>
       </c>
       <c r="J75" s="2">
-        <f t="shared" si="3"/>
+        <f>A75*I75</f>
         <v>0</v>
       </c>
       <c r="K75" s="1" t="s">
@@ -4688,34 +4733,34 @@
         <v>204</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>336</v>
+        <v>189</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="H76" s="3">
-        <v>358</v>
+        <v>267</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>346</v>
       </c>
       <c r="I76" s="2">
-        <v>19.96</v>
+        <v>11.55</v>
       </c>
       <c r="J76" s="2">
         <f>A76*I76</f>
-        <v>0</v>
+        <v>11.55</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>352</v>
@@ -4724,34 +4769,34 @@
         <v>195</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>46</v>
+        <v>339</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>55</v>
+        <v>336</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>53</v>
+        <v>337</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>15</v>
+        <v>338</v>
+      </c>
+      <c r="H77" s="3">
+        <v>358</v>
       </c>
       <c r="I77" s="2">
-        <v>0.28999999999999998</v>
+        <v>19.96</v>
       </c>
       <c r="J77" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>A77*I77</f>
+        <v>19.96</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>203</v>
@@ -4760,34 +4805,34 @@
         <v>239</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>55</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I78" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="J78" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>A78*I78</f>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K78" s="1" t="s">
         <v>203</v>
@@ -4796,7 +4841,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>0</v>
       </c>
@@ -4822,7 +4867,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="J79" s="2">
-        <f t="shared" si="3"/>
+        <f>A79*I79</f>
         <v>0</v>
       </c>
       <c r="K79" s="1" t="s">
@@ -4832,7 +4877,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>0</v>
       </c>
@@ -4868,7 +4913,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>0</v>
       </c>
@@ -4882,7 +4927,7 @@
         <v>0.99</v>
       </c>
       <c r="J81" s="2">
-        <f t="shared" si="3"/>
+        <f>A81*I81</f>
         <v>0</v>
       </c>
       <c r="K81" s="1" t="s">
@@ -4895,9 +4940,9 @@
         <v>323</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>32</v>
@@ -4915,11 +4960,11 @@
         <v>13</v>
       </c>
       <c r="J82" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+        <f>A82*I82</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>0</v>
       </c>
@@ -4945,14 +4990,14 @@
         <v>1.28</v>
       </c>
       <c r="J83" s="2">
-        <f t="shared" si="3"/>
+        <f>A83*I83</f>
         <v>0</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>0</v>
       </c>
@@ -4966,7 +5011,7 @@
         <v>0.15</v>
       </c>
       <c r="J84" s="2">
-        <f t="shared" si="3"/>
+        <f>A84*I84</f>
         <v>0</v>
       </c>
       <c r="K84" s="1" t="s">
@@ -4976,7 +5021,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>0</v>
       </c>
@@ -4990,7 +5035,7 @@
         <v>0.15</v>
       </c>
       <c r="J85" s="2">
-        <f t="shared" si="3"/>
+        <f>A85*I85</f>
         <v>0</v>
       </c>
       <c r="K85" s="1" t="s">
@@ -5000,7 +5045,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>0</v>
       </c>
@@ -5036,7 +5081,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>0</v>
       </c>
@@ -5062,7 +5107,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J87" s="2">
-        <f t="shared" si="3"/>
+        <f>A87*I87</f>
         <v>0</v>
       </c>
       <c r="K87" s="1" t="s">
@@ -5072,7 +5117,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>0</v>
       </c>
@@ -5098,7 +5143,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J88" s="2">
-        <f t="shared" si="3"/>
+        <f>A88*I88</f>
         <v>0</v>
       </c>
       <c r="K88" s="1" t="s">
@@ -5108,7 +5153,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>0</v>
       </c>
@@ -5134,7 +5179,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J89" s="2">
-        <f t="shared" si="3"/>
+        <f>A89*I89</f>
         <v>0</v>
       </c>
       <c r="K89" s="1" t="s">
@@ -5144,7 +5189,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>0</v>
       </c>
@@ -5180,7 +5225,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>0</v>
       </c>
@@ -5206,7 +5251,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J91" s="2">
-        <f t="shared" si="3"/>
+        <f>A91*I91</f>
         <v>0</v>
       </c>
       <c r="K91" s="1" t="s">
@@ -5216,7 +5261,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>0</v>
       </c>
@@ -5252,7 +5297,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>0</v>
       </c>
@@ -5278,7 +5323,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J93" s="2">
-        <f t="shared" si="3"/>
+        <f>A93*I93</f>
         <v>0</v>
       </c>
       <c r="K93" s="1" t="s">
@@ -5288,7 +5333,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>0</v>
       </c>
@@ -5314,7 +5359,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J94" s="2">
-        <f t="shared" si="3"/>
+        <f>A94*I94</f>
         <v>0</v>
       </c>
       <c r="K94" s="1" t="s">
@@ -5324,7 +5369,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>0</v>
       </c>
@@ -5350,7 +5395,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J95" s="2">
-        <f t="shared" si="3"/>
+        <f>A95*I95</f>
         <v>0</v>
       </c>
       <c r="K95" s="1" t="s">
@@ -5360,7 +5405,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>0</v>
       </c>
@@ -5396,7 +5441,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>0</v>
       </c>
@@ -5422,7 +5467,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J97" s="2">
-        <f t="shared" si="3"/>
+        <f>A97*I97</f>
         <v>0</v>
       </c>
       <c r="K97" s="1" t="s">
@@ -5432,7 +5477,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>0</v>
       </c>
@@ -5458,7 +5503,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J98" s="2">
-        <f t="shared" si="3"/>
+        <f>A98*I98</f>
         <v>0</v>
       </c>
       <c r="K98" s="1" t="s">
@@ -5468,7 +5513,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>0</v>
       </c>
@@ -5494,7 +5539,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J99" s="2">
-        <f t="shared" si="3"/>
+        <f>A99*I99</f>
         <v>0</v>
       </c>
       <c r="K99" s="1" t="s">
@@ -5504,7 +5549,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>0</v>
       </c>
@@ -5530,7 +5575,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J100" s="2">
-        <f t="shared" si="3"/>
+        <f>A100*I100</f>
         <v>0</v>
       </c>
       <c r="K100" s="1" t="s">
@@ -5540,7 +5585,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>0</v>
       </c>
@@ -5576,7 +5621,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>0</v>
       </c>
@@ -5602,7 +5647,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J102" s="2">
-        <f t="shared" si="3"/>
+        <f>A102*I102</f>
         <v>0</v>
       </c>
       <c r="K102" s="1" t="s">
@@ -5612,7 +5657,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>0</v>
       </c>
@@ -5648,7 +5693,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>0</v>
       </c>
@@ -5674,7 +5719,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J104" s="2">
-        <f t="shared" si="3"/>
+        <f>A104*I104</f>
         <v>0</v>
       </c>
       <c r="K104" s="1" t="s">
@@ -5684,7 +5729,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>0</v>
       </c>
@@ -5710,7 +5755,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J105" s="2">
-        <f t="shared" si="3"/>
+        <f>A105*I105</f>
         <v>0</v>
       </c>
       <c r="K105" s="1" t="s">
@@ -5720,7 +5765,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>0</v>
       </c>
@@ -5746,7 +5791,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J106" s="2">
-        <f t="shared" si="3"/>
+        <f>A106*I106</f>
         <v>0</v>
       </c>
       <c r="K106" s="1" t="s">
@@ -5756,7 +5801,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>0</v>
       </c>
@@ -5782,7 +5827,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J107" s="2">
-        <f t="shared" si="3"/>
+        <f>A107*I107</f>
         <v>0</v>
       </c>
       <c r="K107" s="1" t="s">
@@ -5792,7 +5837,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>0</v>
       </c>
@@ -5828,7 +5873,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>0</v>
       </c>
@@ -5854,7 +5899,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J109" s="2">
-        <f t="shared" si="3"/>
+        <f>A109*I109</f>
         <v>0</v>
       </c>
       <c r="K109" s="1" t="s">
@@ -5864,7 +5909,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>0</v>
       </c>
@@ -5903,7 +5948,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>0</v>
       </c>
@@ -5929,7 +5974,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J111" s="2">
-        <f t="shared" si="3"/>
+        <f>A111*I111</f>
         <v>0</v>
       </c>
       <c r="K111" s="1" t="s">
@@ -5939,7 +5984,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>0</v>
       </c>
@@ -5965,7 +6010,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J112" s="2">
-        <f t="shared" si="3"/>
+        <f>A112*I112</f>
         <v>0</v>
       </c>
       <c r="K112" s="1" t="s">
@@ -5975,7 +6020,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>0</v>
       </c>
@@ -6001,7 +6046,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J113" s="2">
-        <f t="shared" si="3"/>
+        <f>A113*I113</f>
         <v>0</v>
       </c>
       <c r="K113" s="1" t="s">
@@ -6011,7 +6056,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>0</v>
       </c>
@@ -6037,7 +6082,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J114" s="2">
-        <f t="shared" si="3"/>
+        <f>A114*I114</f>
         <v>0</v>
       </c>
       <c r="K114" s="1" t="s">
@@ -6047,7 +6092,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>0</v>
       </c>
@@ -6083,7 +6128,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>0</v>
       </c>
@@ -6109,7 +6154,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J116" s="2">
-        <f t="shared" si="3"/>
+        <f>A116*I116</f>
         <v>0</v>
       </c>
       <c r="K116" s="1" t="s">
@@ -6119,7 +6164,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>0</v>
       </c>
@@ -6145,7 +6190,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J117" s="2">
-        <f t="shared" ref="J117:J147" si="4">A117*I117</f>
+        <f>A117*I117</f>
         <v>0</v>
       </c>
       <c r="K117" s="1" t="s">
@@ -6155,7 +6200,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>0</v>
       </c>
@@ -6191,7 +6236,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>0</v>
       </c>
@@ -6227,7 +6272,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>0</v>
       </c>
@@ -6253,7 +6298,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J120" s="2">
-        <f t="shared" si="4"/>
+        <f>A120*I120</f>
         <v>0</v>
       </c>
       <c r="K120" s="1" t="s">
@@ -6263,7 +6308,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>0</v>
       </c>
@@ -6289,7 +6334,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J121" s="2">
-        <f t="shared" si="4"/>
+        <f>A121*I121</f>
         <v>0</v>
       </c>
       <c r="K121" s="1" t="s">
@@ -6299,7 +6344,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>0</v>
       </c>
@@ -6325,7 +6370,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J122" s="2">
-        <f t="shared" si="4"/>
+        <f>A122*I122</f>
         <v>0</v>
       </c>
       <c r="K122" s="1" t="s">
@@ -6335,7 +6380,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>0</v>
       </c>
@@ -6361,7 +6406,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J123" s="2">
-        <f t="shared" si="4"/>
+        <f>A123*I123</f>
         <v>0</v>
       </c>
       <c r="K123" s="1" t="s">
@@ -6371,7 +6416,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>0</v>
       </c>
@@ -6407,7 +6452,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>0</v>
       </c>
@@ -6443,7 +6488,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>0</v>
       </c>
@@ -6469,7 +6514,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J126" s="2">
-        <f t="shared" si="4"/>
+        <f>A126*I126</f>
         <v>0</v>
       </c>
       <c r="K126" s="1" t="s">
@@ -6479,7 +6524,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>0</v>
       </c>
@@ -6515,7 +6560,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>0</v>
       </c>
@@ -6551,7 +6596,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>0</v>
       </c>
@@ -6577,7 +6622,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J129" s="2">
-        <f t="shared" si="4"/>
+        <f>A129*I129</f>
         <v>0</v>
       </c>
       <c r="K129" s="1" t="s">
@@ -6587,7 +6632,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>0</v>
       </c>
@@ -6623,7 +6668,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>0</v>
       </c>
@@ -6649,7 +6694,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J131" s="2">
-        <f t="shared" si="4"/>
+        <f>A131*I131</f>
         <v>0</v>
       </c>
       <c r="K131" s="1" t="s">
@@ -6659,7 +6704,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>0</v>
       </c>
@@ -6695,7 +6740,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>0</v>
       </c>
@@ -6731,7 +6776,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>0</v>
       </c>
@@ -6767,7 +6812,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>0</v>
       </c>
@@ -6803,7 +6848,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>0</v>
       </c>
@@ -6839,7 +6884,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>0</v>
       </c>
@@ -6865,7 +6910,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J137" s="2">
-        <f t="shared" si="4"/>
+        <f>A137*I137</f>
         <v>0</v>
       </c>
       <c r="K137" s="1" t="s">
@@ -6875,7 +6920,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>0</v>
       </c>
@@ -6901,7 +6946,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J138" s="2">
-        <f t="shared" si="4"/>
+        <f>A138*I138</f>
         <v>0</v>
       </c>
       <c r="K138" s="1" t="s">
@@ -6911,7 +6956,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>0</v>
       </c>
@@ -6937,7 +6982,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J139" s="2">
-        <f t="shared" si="4"/>
+        <f>A139*I139</f>
         <v>0</v>
       </c>
       <c r="K139" s="1" t="s">
@@ -6947,7 +6992,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>0</v>
       </c>
@@ -6973,7 +7018,7 @@
         <v>0.86</v>
       </c>
       <c r="J140" s="2">
-        <f t="shared" si="4"/>
+        <f>A140*I140</f>
         <v>0</v>
       </c>
       <c r="K140" s="1" t="s">
@@ -6983,7 +7028,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>0</v>
       </c>
@@ -7009,7 +7054,7 @@
         <v>0.17</v>
       </c>
       <c r="J141" s="2">
-        <f t="shared" si="4"/>
+        <f>A141*I141</f>
         <v>0</v>
       </c>
       <c r="K141" s="1" t="s">
@@ -7019,7 +7064,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>0</v>
       </c>
@@ -7039,7 +7084,7 @@
         <v>0.35</v>
       </c>
       <c r="J142" s="2">
-        <f t="shared" si="4"/>
+        <f>A142*I142</f>
         <v>0</v>
       </c>
       <c r="K142" s="1" t="s">
@@ -7049,7 +7094,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>0</v>
       </c>
@@ -7069,7 +7114,7 @@
         <v>0.35</v>
       </c>
       <c r="J143" s="2">
-        <f t="shared" si="4"/>
+        <f>A143*I143</f>
         <v>0</v>
       </c>
       <c r="K143" s="1" t="s">
@@ -7079,7 +7124,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>0</v>
       </c>
@@ -7093,7 +7138,7 @@
         <v>0.85</v>
       </c>
       <c r="J144" s="2">
-        <f t="shared" si="4"/>
+        <f>A144*I144</f>
         <v>0</v>
       </c>
       <c r="K144" s="1" t="s">
@@ -7103,7 +7148,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>0</v>
       </c>
@@ -7129,7 +7174,7 @@
         <v>0.13</v>
       </c>
       <c r="J145" s="2">
-        <f t="shared" si="4"/>
+        <f>A145*I145</f>
         <v>0</v>
       </c>
       <c r="K145" s="1" t="s">
@@ -7142,7 +7187,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>0</v>
       </c>
@@ -7178,7 +7223,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>0</v>
       </c>
@@ -7204,7 +7249,7 @@
         <v>0.67</v>
       </c>
       <c r="J147" s="2">
-        <f t="shared" si="4"/>
+        <f>A147*I147</f>
         <v>0</v>
       </c>
       <c r="K147" s="1" t="s">
@@ -7214,7 +7259,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>0</v>
       </c>
@@ -7247,10 +7292,105 @@
         <v>239</v>
       </c>
     </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A149" s="3">
+        <v>1</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="H149" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="I149" s="2">
+        <v>20</v>
+      </c>
+      <c r="J149" s="2">
+        <f>A149*I149</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A150" s="3">
+        <v>1</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="I150" s="2">
+        <v>0</v>
+      </c>
+      <c r="J150" s="2">
+        <f>A150*I150</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A151" s="3">
+        <v>1</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="I151" s="2">
+        <v>10.88</v>
+      </c>
+      <c r="J151" s="2">
+        <f>A151*I151</f>
+        <v>10.88</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A5:J36" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J84">
-      <sortCondition ref="C5:C38"/>
+  <autoFilter ref="A5:J150" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val="0"/>
+      </customFilters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:J150">
+      <sortCondition descending="1" ref="A5:A150"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -7261,9 +7401,9 @@
     <hyperlink ref="M8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId5"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -7275,16 +7415,16 @@
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="4"/>
+    <col min="1" max="3" width="9.109375" style="4"/>
     <col min="4" max="4" width="28" style="4" customWidth="1"/>
-    <col min="5" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="16.140625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="10" width="9.109375" style="4"/>
+    <col min="11" max="11" width="16.109375" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -7322,7 +7462,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>0</v>
       </c>
@@ -7351,7 +7491,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -7380,7 +7520,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>0</v>
       </c>
@@ -7409,7 +7549,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>0</v>
       </c>
@@ -7438,7 +7578,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -7467,7 +7607,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>0</v>
       </c>
@@ -7491,7 +7631,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>0</v>
       </c>
@@ -7531,128 +7671,128 @@
       <selection activeCell="E18" sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="3"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>

</xml_diff>

<commit_message>
Added remaining footprints and aligned keys on layout
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\ece-445l-final-project-ad_jm_mj_ew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Documents\ECE445L\Lab1\ece-445l-final-project-ad_jm_mj_ew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E357A8DA-18B4-48D9-86EB-6B6E9BE622D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FB9676-2026-41AA-87F6-E454FCA1256C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="543">
   <si>
     <t>Quantity</t>
   </si>
@@ -1707,6 +1707,66 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>MISC</t>
+  </si>
+  <si>
+    <t>Hot-swappable PCB Socket Sip Socket</t>
+  </si>
+  <si>
+    <t>IJKT</t>
+  </si>
+  <si>
+    <t>KS-2P02B01</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0972HB9GY?ref=ppx_yo2ov_dt_b_product_details&amp;th=1</t>
+  </si>
+  <si>
+    <t>TPS73633DBV</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>595-TPS73633DBVRG4</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulators Cap-Free NMOS 400mA</t>
+  </si>
+  <si>
+    <t>POWER</t>
+  </si>
+  <si>
+    <t>TPS2113ADRBR</t>
+  </si>
+  <si>
+    <t>595-TPS2113ADRBR</t>
+  </si>
+  <si>
+    <t>Power Switch IC</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/TPS2113ADRBR?qs=g%2FrhRe7LVpRsXhRevikZ7Q%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/TPS73633DBVRG4?qs=6zVL%252ByCp0mpknSjwGe1Hbg%3D%3D</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
+    <t>ARM Microcontroller</t>
+  </si>
+  <si>
+    <t>TM4C123GH6PMI7</t>
+  </si>
+  <si>
+    <t>595-TM4C123GH6PMI7</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/TM4C123GH6PMI7?qs=m%2F7bTylgptcEEuXHNU46tA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -2286,29 +2346,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:S151"/>
+  <dimension ref="A1:S155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J161" sqref="J161"/>
+      <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="11.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="11.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="18" style="3" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2" customWidth="1"/>
     <col min="11" max="11" width="23" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2326,7 +2386,7 @@
       </c>
       <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>471</v>
       </c>
@@ -2342,7 +2402,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -2354,7 +2414,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>232</v>
       </c>
@@ -2369,10 +2429,10 @@
       </c>
       <c r="J4" s="2">
         <f>SUM(J5:J200)</f>
-        <v>80.83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>106.60000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2410,7 +2470,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -2430,7 +2490,7 @@
         <v>0.6</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" ref="J6:J37" si="0">A6*I6</f>
+        <f t="shared" ref="J6:J34" si="0">A6*I6</f>
         <v>0</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -2443,7 +2503,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -2473,7 +2533,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -2507,7 +2567,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -2540,7 +2600,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -2576,7 +2636,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>0</v>
       </c>
@@ -2609,7 +2669,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>0</v>
       </c>
@@ -2639,7 +2699,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>0</v>
       </c>
@@ -2675,7 +2735,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>0</v>
       </c>
@@ -2705,7 +2765,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>0</v>
       </c>
@@ -2735,7 +2795,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>0</v>
       </c>
@@ -2759,7 +2819,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>0</v>
       </c>
@@ -2789,7 +2849,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>0</v>
       </c>
@@ -2819,7 +2879,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>0</v>
       </c>
@@ -2843,7 +2903,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>0</v>
       </c>
@@ -2867,7 +2927,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>0</v>
       </c>
@@ -2891,7 +2951,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>0</v>
       </c>
@@ -2915,7 +2975,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>0</v>
       </c>
@@ -2939,7 +2999,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>0</v>
       </c>
@@ -2963,7 +3023,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>0</v>
       </c>
@@ -2987,7 +3047,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>0</v>
       </c>
@@ -3026,7 +3086,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>0</v>
       </c>
@@ -3062,7 +3122,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>0</v>
       </c>
@@ -3092,7 +3152,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>0</v>
       </c>
@@ -3122,7 +3182,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>0</v>
       </c>
@@ -3152,7 +3212,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>0</v>
       </c>
@@ -3182,7 +3242,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>0</v>
       </c>
@@ -3212,7 +3272,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>0</v>
       </c>
@@ -3245,7 +3305,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>0</v>
       </c>
@@ -3278,7 +3338,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>65</v>
       </c>
@@ -3304,7 +3364,7 @@
         <v>0.05</v>
       </c>
       <c r="J35" s="2">
-        <f>A35*I35</f>
+        <f t="shared" ref="J35:J56" si="1">A35*I35</f>
         <v>3.25</v>
       </c>
       <c r="K35" s="1" t="s">
@@ -3317,7 +3377,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>0</v>
       </c>
@@ -3343,7 +3403,7 @@
         <v>0.11</v>
       </c>
       <c r="J36" s="2">
-        <f>A36*I36</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K36" s="1" t="s">
@@ -3353,7 +3413,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>0</v>
       </c>
@@ -3379,7 +3439,7 @@
         <v>0.23</v>
       </c>
       <c r="J37" s="2">
-        <f>A37*I37</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K37" s="1" t="s">
@@ -3389,7 +3449,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>0</v>
       </c>
@@ -3415,7 +3475,7 @@
         <v>0.23</v>
       </c>
       <c r="J38" s="2">
-        <f>A38*I38</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K38" s="1" t="s">
@@ -3425,7 +3485,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>0</v>
       </c>
@@ -3451,7 +3511,7 @@
         <v>0.23</v>
       </c>
       <c r="J39" s="2">
-        <f>A39*I39</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K39" s="1" t="s">
@@ -3461,7 +3521,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>0</v>
       </c>
@@ -3487,7 +3547,7 @@
         <v>0.23</v>
       </c>
       <c r="J40" s="2">
-        <f>A40*I40</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K40" s="1" t="s">
@@ -3497,7 +3557,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>0</v>
       </c>
@@ -3523,7 +3583,7 @@
         <v>0.23</v>
       </c>
       <c r="J41" s="2">
-        <f>A41*I41</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K41" s="1" t="s">
@@ -3533,7 +3593,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>0</v>
       </c>
@@ -3559,7 +3619,7 @@
         <v>0.23</v>
       </c>
       <c r="J42" s="2">
-        <f>A42*I42</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K42" s="1" t="s">
@@ -3569,7 +3629,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>0</v>
       </c>
@@ -3595,7 +3655,7 @@
         <v>0.23</v>
       </c>
       <c r="J43" s="2">
-        <f>A43*I43</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K43" s="1" t="s">
@@ -3605,7 +3665,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>0</v>
       </c>
@@ -3631,14 +3691,14 @@
         <v>1.98</v>
       </c>
       <c r="J44" s="2">
-        <f>A44*I44</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>0</v>
       </c>
@@ -3664,7 +3724,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="J45" s="2">
-        <f>A45*I45</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K45" s="1" t="s">
@@ -3677,7 +3737,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>0</v>
       </c>
@@ -3703,7 +3763,7 @@
         <v>2.46</v>
       </c>
       <c r="J46" s="2">
-        <f>A46*I46</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K46" s="1" t="s">
@@ -3713,7 +3773,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>3</v>
       </c>
@@ -3739,7 +3799,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="J47" s="2">
-        <f>A47*I47</f>
+        <f t="shared" si="1"/>
         <v>0.86999999999999988</v>
       </c>
       <c r="K47" s="1" t="s">
@@ -3749,7 +3809,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>0</v>
       </c>
@@ -3775,7 +3835,7 @@
         <v>0.65</v>
       </c>
       <c r="J48" s="2">
-        <f>A48*I48</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K48" s="1" t="s">
@@ -3785,7 +3845,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="49" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>0</v>
       </c>
@@ -3811,7 +3871,7 @@
         <v>0.26</v>
       </c>
       <c r="J49" s="2">
-        <f>A49*I49</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K49" s="1" t="s">
@@ -3821,7 +3881,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>0</v>
       </c>
@@ -3847,7 +3907,7 @@
         <v>0.27</v>
       </c>
       <c r="J50" s="2">
-        <f>A50*I50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K50" s="1" t="s">
@@ -3857,7 +3917,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>1</v>
       </c>
@@ -3877,7 +3937,7 @@
         <v>0.27</v>
       </c>
       <c r="J51" s="2">
-        <f>A51*I51</f>
+        <f t="shared" si="1"/>
         <v>0.27</v>
       </c>
       <c r="K51" s="1" t="s">
@@ -3887,7 +3947,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="52" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>0</v>
       </c>
@@ -3913,7 +3973,7 @@
         <v>2.7</v>
       </c>
       <c r="J52" s="2">
-        <f>A52*I52</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K52" s="1" t="s">
@@ -3923,7 +3983,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>1</v>
       </c>
@@ -3949,7 +4009,7 @@
         <v>0.47</v>
       </c>
       <c r="J53" s="2">
-        <f>A53*I53</f>
+        <f t="shared" si="1"/>
         <v>0.47</v>
       </c>
       <c r="K53" s="1" t="s">
@@ -3959,7 +4019,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>0</v>
       </c>
@@ -3985,7 +4045,7 @@
         <v>0.51</v>
       </c>
       <c r="J54" s="2">
-        <f>A54*I54</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K54" s="3" t="s">
@@ -3998,7 +4058,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>1</v>
       </c>
@@ -4012,7 +4072,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="J55" s="2">
-        <f>A55*I55</f>
+        <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="K55" s="1" t="s">
@@ -4022,7 +4082,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>0</v>
       </c>
@@ -4048,7 +4108,7 @@
         <v>1.17</v>
       </c>
       <c r="J56" s="2">
-        <f>A56*I56</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K56" s="1" t="s">
@@ -4058,7 +4118,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="57" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>0</v>
       </c>
@@ -4094,7 +4154,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="58" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>0</v>
       </c>
@@ -4120,7 +4180,7 @@
         <v>0.19</v>
       </c>
       <c r="J58" s="2">
-        <f>A58*I58</f>
+        <f t="shared" ref="J58:J89" si="2">A58*I58</f>
         <v>0</v>
       </c>
       <c r="K58" s="1" t="s">
@@ -4130,7 +4190,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="59" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>0</v>
       </c>
@@ -4156,7 +4216,7 @@
         <v>12.15</v>
       </c>
       <c r="J59" s="2">
-        <f>A59*I59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K59" s="1" t="s">
@@ -4166,7 +4226,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>0</v>
       </c>
@@ -4192,7 +4252,7 @@
         <v>10.09</v>
       </c>
       <c r="J60" s="2">
-        <f>A60*I60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K60" s="3" t="s">
@@ -4202,7 +4262,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>0</v>
       </c>
@@ -4228,7 +4288,7 @@
         <v>14.18</v>
       </c>
       <c r="J61" s="2">
-        <f>A61*I61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K61" s="3" t="s">
@@ -4238,7 +4298,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>0</v>
       </c>
@@ -4264,7 +4324,7 @@
         <v>9.09</v>
       </c>
       <c r="J62" s="2">
-        <f>A62*I62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K62" s="1" t="s">
@@ -4274,7 +4334,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="63" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>0</v>
       </c>
@@ -4294,7 +4354,7 @@
         <v>492</v>
       </c>
       <c r="J63" s="2">
-        <f>A63*I63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K63" s="3" t="s">
@@ -4307,7 +4367,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="64" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>0</v>
       </c>
@@ -4333,7 +4393,7 @@
         <v>3.06</v>
       </c>
       <c r="J64" s="2">
-        <f>A64*I64</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K64" s="1" t="s">
@@ -4346,7 +4406,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="65" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>0</v>
       </c>
@@ -4372,7 +4432,7 @@
         <v>2.9</v>
       </c>
       <c r="J65" s="2">
-        <f>A65*I65</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K65" s="1" t="s">
@@ -4385,7 +4445,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="66" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>0</v>
       </c>
@@ -4411,7 +4471,7 @@
         <v>2.31</v>
       </c>
       <c r="J66" s="2">
-        <f>A66*I66</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K66" s="1" t="s">
@@ -4424,7 +4484,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>0</v>
       </c>
@@ -4450,7 +4510,7 @@
         <v>1.21</v>
       </c>
       <c r="J67" s="2">
-        <f>A67*I67</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K67" s="1" t="s">
@@ -4463,7 +4523,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>0</v>
       </c>
@@ -4489,7 +4549,7 @@
         <v>3.5</v>
       </c>
       <c r="J68" s="2">
-        <f>A68*I68</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K68" s="1" t="s">
@@ -4502,7 +4562,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>0</v>
       </c>
@@ -4522,7 +4582,7 @@
         <v>0.4</v>
       </c>
       <c r="J69" s="2">
-        <f>A69*I69</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L69" s="1" t="s">
@@ -4532,7 +4592,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>0</v>
       </c>
@@ -4552,7 +4612,7 @@
         <v>0.3</v>
       </c>
       <c r="J70" s="2">
-        <f>A70*I70</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L70" s="1" t="s">
@@ -4562,7 +4622,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="71" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>0</v>
       </c>
@@ -4588,14 +4648,14 @@
         <v>0.53</v>
       </c>
       <c r="J71" s="2">
-        <f>A71*I71</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="72" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>0</v>
       </c>
@@ -4621,7 +4681,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="J72" s="2">
-        <f>A72*I72</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K72" s="1" t="s">
@@ -4634,7 +4694,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="73" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>0</v>
       </c>
@@ -4654,7 +4714,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J73" s="2">
-        <f>A73*I73</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K73" s="1" t="s">
@@ -4667,7 +4727,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="74" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>0</v>
       </c>
@@ -4687,7 +4747,7 @@
         <v>0.09</v>
       </c>
       <c r="J74" s="2">
-        <f>A74*I74</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K74" s="1" t="s">
@@ -4700,7 +4760,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>0</v>
       </c>
@@ -4720,7 +4780,7 @@
         <v>2.99</v>
       </c>
       <c r="J75" s="2">
-        <f>A75*I75</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K75" s="1" t="s">
@@ -4733,7 +4793,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>1</v>
       </c>
@@ -4759,7 +4819,7 @@
         <v>11.55</v>
       </c>
       <c r="J76" s="2">
-        <f>A76*I76</f>
+        <f t="shared" si="2"/>
         <v>11.55</v>
       </c>
       <c r="K76" s="1" t="s">
@@ -4769,7 +4829,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>1</v>
       </c>
@@ -4795,7 +4855,7 @@
         <v>19.96</v>
       </c>
       <c r="J77" s="2">
-        <f>A77*I77</f>
+        <f t="shared" si="2"/>
         <v>19.96</v>
       </c>
       <c r="K77" s="1" t="s">
@@ -4805,7 +4865,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>1</v>
       </c>
@@ -4831,7 +4891,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="J78" s="2">
-        <f>A78*I78</f>
+        <f t="shared" si="2"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="K78" s="1" t="s">
@@ -4841,7 +4901,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="79" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>0</v>
       </c>
@@ -4867,7 +4927,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="J79" s="2">
-        <f>A79*I79</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K79" s="1" t="s">
@@ -4877,7 +4937,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="80" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>0</v>
       </c>
@@ -4903,7 +4963,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="J80" s="2">
-        <f>A80*I80</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K80" s="1" t="s">
@@ -4913,7 +4973,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>0</v>
       </c>
@@ -4927,7 +4987,7 @@
         <v>0.99</v>
       </c>
       <c r="J81" s="2">
-        <f>A81*I81</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K81" s="1" t="s">
@@ -4940,7 +5000,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>1</v>
       </c>
@@ -4960,11 +5020,11 @@
         <v>13</v>
       </c>
       <c r="J82" s="2">
-        <f>A82*I82</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>0</v>
       </c>
@@ -4990,14 +5050,14 @@
         <v>1.28</v>
       </c>
       <c r="J83" s="2">
-        <f>A83*I83</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>0</v>
       </c>
@@ -5011,7 +5071,7 @@
         <v>0.15</v>
       </c>
       <c r="J84" s="2">
-        <f>A84*I84</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K84" s="1" t="s">
@@ -5021,7 +5081,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>0</v>
       </c>
@@ -5035,7 +5095,7 @@
         <v>0.15</v>
       </c>
       <c r="J85" s="2">
-        <f>A85*I85</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K85" s="1" t="s">
@@ -5045,7 +5105,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>0</v>
       </c>
@@ -5071,7 +5131,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J86" s="2">
-        <f>A86*I86</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K86" s="1" t="s">
@@ -5081,7 +5141,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>0</v>
       </c>
@@ -5107,7 +5167,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J87" s="2">
-        <f>A87*I87</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K87" s="1" t="s">
@@ -5117,7 +5177,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>0</v>
       </c>
@@ -5143,7 +5203,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J88" s="2">
-        <f>A88*I88</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K88" s="1" t="s">
@@ -5153,7 +5213,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>0</v>
       </c>
@@ -5179,7 +5239,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J89" s="2">
-        <f>A89*I89</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K89" s="1" t="s">
@@ -5189,7 +5249,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>0</v>
       </c>
@@ -5215,7 +5275,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J90" s="2">
-        <f>A90*I90</f>
+        <f t="shared" ref="J90:J121" si="3">A90*I90</f>
         <v>0</v>
       </c>
       <c r="K90" s="1" t="s">
@@ -5225,7 +5285,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>0</v>
       </c>
@@ -5251,7 +5311,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J91" s="2">
-        <f>A91*I91</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K91" s="1" t="s">
@@ -5261,7 +5321,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>0</v>
       </c>
@@ -5287,7 +5347,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J92" s="2">
-        <f>A92*I92</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K92" s="1" t="s">
@@ -5297,7 +5357,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>0</v>
       </c>
@@ -5323,7 +5383,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J93" s="2">
-        <f>A93*I93</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K93" s="1" t="s">
@@ -5333,7 +5393,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>0</v>
       </c>
@@ -5359,7 +5419,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J94" s="2">
-        <f>A94*I94</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K94" s="1" t="s">
@@ -5369,7 +5429,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>0</v>
       </c>
@@ -5395,7 +5455,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J95" s="2">
-        <f>A95*I95</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K95" s="1" t="s">
@@ -5405,7 +5465,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>0</v>
       </c>
@@ -5431,7 +5491,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J96" s="2">
-        <f>A96*I96</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K96" s="1" t="s">
@@ -5441,7 +5501,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>0</v>
       </c>
@@ -5467,7 +5527,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J97" s="2">
-        <f>A97*I97</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K97" s="1" t="s">
@@ -5477,7 +5537,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>0</v>
       </c>
@@ -5503,7 +5563,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J98" s="2">
-        <f>A98*I98</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K98" s="1" t="s">
@@ -5513,7 +5573,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>0</v>
       </c>
@@ -5539,7 +5599,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J99" s="2">
-        <f>A99*I99</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K99" s="1" t="s">
@@ -5549,7 +5609,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>0</v>
       </c>
@@ -5575,7 +5635,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J100" s="2">
-        <f>A100*I100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K100" s="1" t="s">
@@ -5585,7 +5645,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>0</v>
       </c>
@@ -5611,7 +5671,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J101" s="2">
-        <f>A101*I101</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K101" s="1" t="s">
@@ -5621,7 +5681,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>0</v>
       </c>
@@ -5647,7 +5707,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J102" s="2">
-        <f>A102*I102</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K102" s="1" t="s">
@@ -5657,7 +5717,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>0</v>
       </c>
@@ -5683,7 +5743,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J103" s="2">
-        <f>A103*I103</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K103" s="1" t="s">
@@ -5693,7 +5753,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>0</v>
       </c>
@@ -5719,7 +5779,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J104" s="2">
-        <f>A104*I104</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K104" s="1" t="s">
@@ -5729,7 +5789,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>0</v>
       </c>
@@ -5755,7 +5815,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J105" s="2">
-        <f>A105*I105</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K105" s="1" t="s">
@@ -5765,7 +5825,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>0</v>
       </c>
@@ -5791,7 +5851,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J106" s="2">
-        <f>A106*I106</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K106" s="1" t="s">
@@ -5801,7 +5861,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>0</v>
       </c>
@@ -5827,7 +5887,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J107" s="2">
-        <f>A107*I107</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K107" s="1" t="s">
@@ -5837,7 +5897,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>0</v>
       </c>
@@ -5863,7 +5923,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J108" s="2">
-        <f>A108*I108</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K108" s="1" t="s">
@@ -5873,7 +5933,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>0</v>
       </c>
@@ -5899,7 +5959,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J109" s="2">
-        <f>A109*I109</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K109" s="1" t="s">
@@ -5909,7 +5969,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>0</v>
       </c>
@@ -5935,7 +5995,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J110" s="2">
-        <f>A110*I110</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K110" s="1" t="s">
@@ -5948,7 +6008,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>0</v>
       </c>
@@ -5974,7 +6034,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J111" s="2">
-        <f>A111*I111</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K111" s="1" t="s">
@@ -5984,7 +6044,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>0</v>
       </c>
@@ -6010,7 +6070,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J112" s="2">
-        <f>A112*I112</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K112" s="1" t="s">
@@ -6020,7 +6080,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>0</v>
       </c>
@@ -6046,7 +6106,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J113" s="2">
-        <f>A113*I113</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K113" s="1" t="s">
@@ -6056,7 +6116,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>0</v>
       </c>
@@ -6082,7 +6142,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J114" s="2">
-        <f>A114*I114</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K114" s="1" t="s">
@@ -6092,7 +6152,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>0</v>
       </c>
@@ -6118,7 +6178,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J115" s="2">
-        <f>A115*I115</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K115" s="1" t="s">
@@ -6128,7 +6188,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>0</v>
       </c>
@@ -6154,7 +6214,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J116" s="2">
-        <f>A116*I116</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K116" s="1" t="s">
@@ -6164,7 +6224,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>0</v>
       </c>
@@ -6190,7 +6250,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J117" s="2">
-        <f>A117*I117</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K117" s="1" t="s">
@@ -6200,7 +6260,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>0</v>
       </c>
@@ -6226,7 +6286,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J118" s="2">
-        <f>A118*I118</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K118" s="1" t="s">
@@ -6236,7 +6296,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>0</v>
       </c>
@@ -6262,7 +6322,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J119" s="2">
-        <f>A119*I119</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K119" s="1" t="s">
@@ -6272,7 +6332,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>0</v>
       </c>
@@ -6298,7 +6358,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J120" s="2">
-        <f>A120*I120</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K120" s="1" t="s">
@@ -6308,7 +6368,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>0</v>
       </c>
@@ -6334,7 +6394,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J121" s="2">
-        <f>A121*I121</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K121" s="1" t="s">
@@ -6344,7 +6404,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>0</v>
       </c>
@@ -6370,7 +6430,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J122" s="2">
-        <f>A122*I122</f>
+        <f t="shared" ref="J122:J155" si="4">A122*I122</f>
         <v>0</v>
       </c>
       <c r="K122" s="1" t="s">
@@ -6380,7 +6440,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>0</v>
       </c>
@@ -6406,7 +6466,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J123" s="2">
-        <f>A123*I123</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K123" s="1" t="s">
@@ -6416,7 +6476,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>0</v>
       </c>
@@ -6442,7 +6502,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J124" s="2">
-        <f>A124*I124</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K124" s="1" t="s">
@@ -6452,7 +6512,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>0</v>
       </c>
@@ -6478,7 +6538,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J125" s="2">
-        <f>A125*I125</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K125" s="1" t="s">
@@ -6488,7 +6548,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>0</v>
       </c>
@@ -6514,7 +6574,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J126" s="2">
-        <f>A126*I126</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K126" s="1" t="s">
@@ -6524,7 +6584,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>0</v>
       </c>
@@ -6550,7 +6610,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J127" s="2">
-        <f>A127*I127</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K127" s="1" t="s">
@@ -6560,7 +6620,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>0</v>
       </c>
@@ -6586,7 +6646,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J128" s="2">
-        <f>A128*I128</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K128" s="1" t="s">
@@ -6596,7 +6656,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>0</v>
       </c>
@@ -6622,7 +6682,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J129" s="2">
-        <f>A129*I129</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K129" s="1" t="s">
@@ -6632,7 +6692,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>0</v>
       </c>
@@ -6658,7 +6718,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J130" s="2">
-        <f>A130*I130</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K130" s="1" t="s">
@@ -6668,7 +6728,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>0</v>
       </c>
@@ -6694,7 +6754,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J131" s="2">
-        <f>A131*I131</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K131" s="1" t="s">
@@ -6704,7 +6764,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>0</v>
       </c>
@@ -6730,7 +6790,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J132" s="2">
-        <f>A132*I132</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K132" s="1" t="s">
@@ -6740,7 +6800,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>0</v>
       </c>
@@ -6766,7 +6826,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J133" s="2">
-        <f>A133*I133</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K133" s="1" t="s">
@@ -6776,7 +6836,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>0</v>
       </c>
@@ -6802,7 +6862,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J134" s="2">
-        <f>A134*I134</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K134" s="1" t="s">
@@ -6812,7 +6872,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>0</v>
       </c>
@@ -6838,7 +6898,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J135" s="2">
-        <f>A135*I135</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K135" s="1" t="s">
@@ -6848,7 +6908,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>0</v>
       </c>
@@ -6874,7 +6934,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J136" s="2">
-        <f>A136*I136</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K136" s="1" t="s">
@@ -6884,7 +6944,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>0</v>
       </c>
@@ -6910,7 +6970,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J137" s="2">
-        <f>A137*I137</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K137" s="1" t="s">
@@ -6920,7 +6980,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>0</v>
       </c>
@@ -6946,7 +7006,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J138" s="2">
-        <f>A138*I138</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K138" s="1" t="s">
@@ -6956,7 +7016,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>0</v>
       </c>
@@ -6982,7 +7042,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J139" s="2">
-        <f>A139*I139</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K139" s="1" t="s">
@@ -6992,7 +7052,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>0</v>
       </c>
@@ -7018,7 +7078,7 @@
         <v>0.86</v>
       </c>
       <c r="J140" s="2">
-        <f>A140*I140</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K140" s="1" t="s">
@@ -7028,7 +7088,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>0</v>
       </c>
@@ -7054,7 +7114,7 @@
         <v>0.17</v>
       </c>
       <c r="J141" s="2">
-        <f>A141*I141</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K141" s="1" t="s">
@@ -7064,7 +7124,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>0</v>
       </c>
@@ -7084,7 +7144,7 @@
         <v>0.35</v>
       </c>
       <c r="J142" s="2">
-        <f>A142*I142</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K142" s="1" t="s">
@@ -7094,7 +7154,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>0</v>
       </c>
@@ -7114,7 +7174,7 @@
         <v>0.35</v>
       </c>
       <c r="J143" s="2">
-        <f>A143*I143</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K143" s="1" t="s">
@@ -7124,7 +7184,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>0</v>
       </c>
@@ -7138,7 +7198,7 @@
         <v>0.85</v>
       </c>
       <c r="J144" s="2">
-        <f>A144*I144</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K144" s="1" t="s">
@@ -7148,7 +7208,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>0</v>
       </c>
@@ -7174,7 +7234,7 @@
         <v>0.13</v>
       </c>
       <c r="J145" s="2">
-        <f>A145*I145</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K145" s="1" t="s">
@@ -7187,7 +7247,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>0</v>
       </c>
@@ -7213,7 +7273,7 @@
         <v>0.68</v>
       </c>
       <c r="J146" s="2">
-        <f>A146*I146</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K146" s="1" t="s">
@@ -7223,7 +7283,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>0</v>
       </c>
@@ -7249,7 +7309,7 @@
         <v>0.67</v>
       </c>
       <c r="J147" s="2">
-        <f>A147*I147</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K147" s="1" t="s">
@@ -7259,7 +7319,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>0</v>
       </c>
@@ -7282,7 +7342,7 @@
         <v>1.95</v>
       </c>
       <c r="J148" s="2">
-        <f>A148*I148</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K148" s="1" t="s">
@@ -7292,7 +7352,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>1</v>
       </c>
@@ -7318,11 +7378,11 @@
         <v>20</v>
       </c>
       <c r="J149" s="2">
-        <f>A149*I149</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>1</v>
       </c>
@@ -7348,11 +7408,11 @@
         <v>0</v>
       </c>
       <c r="J150" s="2">
-        <f>A150*I150</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>1</v>
       </c>
@@ -7378,8 +7438,137 @@
         <v>10.88</v>
       </c>
       <c r="J151" s="2">
-        <f>A151*I151</f>
+        <f t="shared" si="4"/>
         <v>10.88</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A152" s="3">
+        <v>1</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="I152" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="J152" s="2">
+        <f t="shared" si="4"/>
+        <v>9.9</v>
+      </c>
+      <c r="L152" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A153" s="3">
+        <v>1</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="I153" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J153" s="2">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="L153" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A154" s="3">
+        <v>1</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I154" s="2">
+        <v>1.87</v>
+      </c>
+      <c r="J154" s="2">
+        <f t="shared" si="4"/>
+        <v>1.87</v>
+      </c>
+      <c r="L154" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A155" s="3">
+        <v>1</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="H155" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="I155" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="J155" s="2">
+        <f t="shared" si="4"/>
+        <v>12.5</v>
+      </c>
+      <c r="L155" s="1" t="s">
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -7415,16 +7604,16 @@
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9.109375" style="4"/>
+    <col min="1" max="3" width="9.140625" style="4"/>
     <col min="4" max="4" width="28" style="4" customWidth="1"/>
-    <col min="5" max="10" width="9.109375" style="4"/>
-    <col min="11" max="11" width="16.109375" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="4"/>
+    <col min="5" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="16.140625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -7462,7 +7651,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>0</v>
       </c>
@@ -7491,7 +7680,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -7520,7 +7709,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>0</v>
       </c>
@@ -7549,7 +7738,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>0</v>
       </c>
@@ -7578,7 +7767,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -7607,7 +7796,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>0</v>
       </c>
@@ -7631,7 +7820,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>0</v>
       </c>
@@ -7671,128 +7860,128 @@
       <selection activeCell="E18" sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="3"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>

</xml_diff>

<commit_message>
Verified regulator circuit, added LEDs based on BOM
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Documents\ECE445L\Lab1\ece-445l-final-project-ad_jm_mj_ew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Repositories\ece-445l-final-project-ad_jm_mj_ew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FB9676-2026-41AA-87F6-E454FCA1256C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673E4E75-6FFE-471F-8712-83B1B0BE7C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40170" yWindow="2655" windowWidth="31755" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -1712,9 +1712,6 @@
     <t>MISC</t>
   </si>
   <si>
-    <t>Hot-swappable PCB Socket Sip Socket</t>
-  </si>
-  <si>
     <t>IJKT</t>
   </si>
   <si>
@@ -1767,6 +1764,9 @@
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/Texas-Instruments/TM4C123GH6PMI7?qs=m%2F7bTylgptcEEuXHNU46tA%3D%3D</t>
+  </si>
+  <si>
+    <t>Hot-swappable PCB Socket Sip Socket x70</t>
   </si>
 </sst>
 </file>
@@ -2350,7 +2350,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
+      <selection pane="bottomLeft" activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7450,13 +7450,13 @@
         <v>523</v>
       </c>
       <c r="D152" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="E152" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="E152" s="3" t="s">
+      <c r="F152" s="3" t="s">
         <v>525</v>
-      </c>
-      <c r="F152" s="3" t="s">
-        <v>526</v>
       </c>
       <c r="G152" s="3" t="s">
         <v>513</v>
@@ -7469,7 +7469,7 @@
         <v>9.9</v>
       </c>
       <c r="L152" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
@@ -7477,22 +7477,22 @@
         <v>1</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G153" s="3" t="s">
         <v>267</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I153" s="2">
         <v>1.5</v>
@@ -7502,7 +7502,7 @@
         <v>1.5</v>
       </c>
       <c r="L153" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -7510,22 +7510,22 @@
         <v>1</v>
       </c>
       <c r="C154" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="F154" s="3" t="s">
         <v>532</v>
-      </c>
-      <c r="D154" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="F154" s="3" t="s">
-        <v>533</v>
       </c>
       <c r="G154" s="3" t="s">
         <v>267</v>
       </c>
       <c r="H154" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I154" s="2">
         <v>1.87</v>
@@ -7535,7 +7535,7 @@
         <v>1.87</v>
       </c>
       <c r="L154" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
@@ -7543,22 +7543,22 @@
         <v>1</v>
       </c>
       <c r="C155" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="D155" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="E155" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="F155" s="3" t="s">
         <v>539</v>
-      </c>
-      <c r="E155" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="F155" s="3" t="s">
-        <v>540</v>
       </c>
       <c r="G155" s="3" t="s">
         <v>267</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I155" s="2">
         <v>12.5</v>
@@ -7568,7 +7568,7 @@
         <v>12.5</v>
       </c>
       <c r="L155" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verified TM4C pin #s and important pins, MOSC, and caps
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Repositories\ece-445l-final-project-ad_jm_mj_ew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673E4E75-6FFE-471F-8712-83B1B0BE7C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15149A4C-883D-4E14-93DB-1386A1B54189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40170" yWindow="2655" windowWidth="31755" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$5:$J$150</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$5:$J$155</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2349,8 +2349,8 @@
   <dimension ref="A1:S155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F149" sqref="F149"/>
+      <pane ySplit="5" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G159" sqref="G159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="J4" s="2">
         <f>SUM(J5:J200)</f>
-        <v>106.60000000000001</v>
+        <v>107.73</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3047,9 +3047,9 @@
         <v>239</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>25</v>
@@ -3074,7 +3074,7 @@
       </c>
       <c r="J26" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>182</v>
@@ -4019,9 +4019,9 @@
         <v>465</v>
       </c>
     </row>
-    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>223</v>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="J54" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="K54" s="3" t="s">
         <v>351</v>
@@ -4144,7 +4144,7 @@
         <v>0.19</v>
       </c>
       <c r="J57" s="2">
-        <f>A58*I57</f>
+        <f>A57*I57</f>
         <v>0</v>
       </c>
       <c r="K57" s="1" t="s">
@@ -7572,11 +7572,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:J150" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A5:J155" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="notEqual" val="0"/>
-      </customFilters>
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+        <filter val="3"/>
+        <filter val="65"/>
+      </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:J150">
       <sortCondition descending="1" ref="A5:A150"/>

</xml_diff>

<commit_message>
Updated BoM to include LEDs and M2x4 mounting screws.
Length of screws can be updated depending on the thickness of the PCB

Also updated resistor values based on forward voltage of SMD LEDs
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Repositories\ece-445l-final-project-ad_jm_mj_ew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Documents\ECE445L\Lab1\ece-445l-final-project-ad_jm_mj_ew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E49C36-8BCC-44D3-AA3D-207EE8C0FC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9318DD83-A682-4206-9D61-0328878507F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40515" yWindow="3870" windowWidth="31755" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="579">
   <si>
     <t>Quantity</t>
   </si>
@@ -1848,6 +1848,33 @@
   </si>
   <si>
     <t>https://www.amazon.com/dp/B0BV2CKDJW?psc=1&amp;smid=A3HH0O874SI0OR</t>
+  </si>
+  <si>
+    <t>SCREW</t>
+  </si>
+  <si>
+    <t>10-pack M2 x 4 mm flat-head screws</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Deal4GO-10-Pack-Replacement-Phillips-Heatsink/dp/B0B373RNJP/ref=sr_1_2?keywords=M2%2Bx%2B4mm%2Bflat%2Bhead%2Bscrew&amp;sr=8-2&amp;th=1</t>
+  </si>
+  <si>
+    <t>LED RED CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
+    <t>APTD1608SEC/J3</t>
+  </si>
+  <si>
+    <t>604-APTD1608SEC/J3</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Kingbright/APTD1608SEC-J3?qs=6pLj%252BqlhfwAhstDKTOglEA%3D%3D</t>
+  </si>
+  <si>
+    <t>Generic</t>
   </si>
 </sst>
 </file>
@@ -2427,11 +2454,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:S163"/>
+  <dimension ref="A1:S165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G166" sqref="G166"/>
+      <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A165" sqref="A165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2509,8 +2536,8 @@
         <v>514</v>
       </c>
       <c r="J4" s="2">
-        <f>SUM(J5:J198)</f>
-        <v>140.90000000000003</v>
+        <f>SUM(J5:J197)</f>
+        <v>147.05000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -6439,7 +6466,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="J120" s="2">
-        <f t="shared" ref="J120:J163" si="4">A120*I120</f>
+        <f t="shared" ref="J120:J164" si="4">A120*I120</f>
         <v>0</v>
       </c>
       <c r="K120" s="1" t="s">
@@ -7854,6 +7881,66 @@
       </c>
       <c r="L163" s="1" t="s">
         <v>568</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A164" s="3">
+        <v>3</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="H164" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="I164" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="J164" s="2">
+        <f t="shared" si="4"/>
+        <v>2.16</v>
+      </c>
+      <c r="L164" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A165" s="3">
+        <v>1</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="I165" s="2">
+        <v>3.99</v>
+      </c>
+      <c r="J165" s="2">
+        <f t="shared" ref="J165" si="5">A165*I165</f>
+        <v>3.99</v>
+      </c>
+      <c r="L165" s="1" t="s">
+        <v>572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some basic unit testing procedures (for lab 8 report) for once pcb arrives
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Documents\ECE445L\Lab1\ece-445l-final-project-ad_jm_mj_ew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9318DD83-A682-4206-9D61-0328878507F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B900F744-E3A0-4425-BA97-74B22BE582BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2457,8 +2457,8 @@
   <dimension ref="A1:S165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A165" sqref="A165"/>
+      <pane ySplit="5" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H157" sqref="H157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="J4" s="2">
         <f>SUM(J5:J197)</f>
-        <v>147.05000000000004</v>
+        <v>171.04</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -5053,11 +5053,11 @@
         <v>473</v>
       </c>
       <c r="I80" s="2">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J80" s="2">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
@@ -7918,7 +7918,7 @@
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>570</v>
@@ -7937,7 +7937,7 @@
       </c>
       <c r="J165" s="2">
         <f t="shared" ref="J165" si="5">A165*I165</f>
-        <v>3.99</v>
+        <v>7.98</v>
       </c>
       <c r="L165" s="1" t="s">
         <v>572</v>

</xml_diff>